<commit_message>
se elimino el boton de carga de archivo y se dejo automatico al buscar
</commit_message>
<xml_diff>
--- a/uploads/Calificaciones.xlsx
+++ b/uploads/Calificaciones.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\proyectos\GITHUB\GraficaCalificaciones\uploads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documentos\Proyectos\test\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65DF8D37-10CB-4A5A-887A-6A4B9DBC1085}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7665"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -144,7 +143,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -536,11 +535,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="F11" sqref="A11:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>